<commit_message>
Writes the received stream on LoggingNormon.xlsx
</commit_message>
<xml_diff>
--- a/Ed_FInsOmron/resources/LoggingNormon.xlsx
+++ b/Ed_FInsOmron/resources/LoggingNormon.xlsx
@@ -3,59 +3,69 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4525363D-6488-4DC9-A2BD-5F7967700B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{354394A5-112B-4FEC-AF5A-EE55FE182FB1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
-  <si>
-    <t>DataV10</t>
-  </si>
-  <si>
-    <t>Codigo_Caja</t>
-  </si>
-  <si>
-    <t>Hojas_Totales</t>
-  </si>
-  <si>
-    <t>Hojas_Leer</t>
-  </si>
-  <si>
-    <t>NºMáquina</t>
-  </si>
-  <si>
-    <t>Resultado_Lectura</t>
-  </si>
-  <si>
-    <t>DataSunt Alb_1</t>
-  </si>
-  <si>
-    <t>DataSunt Alb_2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">DataV10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo_Caja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hojas_Totales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hojas_Leer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NºMáquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado_Lectura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataSunt Alb_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataSunt Alb_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trama_Completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450000217702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450000217702020201d0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +75,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -152,22 +170,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,11 +202,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -481,71 +508,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B429635C-8ABC-47A3-9119-BA69E8A34554}">
-  <dimension ref="B1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="B1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="H2" s="1" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="5"/>
+      <c r="N2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="O3" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ip and port Changes || now the received data and sended data keeps write in excel doc, still remains to do to write sendedData From plc2
</commit_message>
<xml_diff>
--- a/Ed_FInsOmron/resources/LoggingNormon.xlsx
+++ b/Ed_FInsOmron/resources/LoggingNormon.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t xml:space="preserve">DataV10</t>
   </si>
@@ -48,16 +48,22 @@
     <t xml:space="preserve">Trama_Completa</t>
   </si>
   <si>
-    <t xml:space="preserve">184123450000217702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">184123450000217702020201d0</t>
+    <t xml:space="preserve">18412345000217701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23138343132333435303030323137373031303330333d00000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450000171300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345000017130000000000</t>
   </si>
 </sst>
 </file>
@@ -172,20 +178,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -193,6 +187,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="B1:O5"/>
+  <dimension ref="B1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,51 +526,58 @@
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.21875" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="J2" s="4" t="s">
+      <c r="F2" s="7"/>
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="N2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="5"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>1</v>
@@ -574,165 +585,41 @@
       <c r="O3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="P3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="N2:O2"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implements the ExcelWriter class. Use array List to save the part of the stream . The cycle that call to the method to write not found.
</commit_message>
<xml_diff>
--- a/Ed_FInsOmron/resources/LoggingNormon.xlsx
+++ b/Ed_FInsOmron/resources/LoggingNormon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t xml:space="preserve">DataV10</t>
   </si>
@@ -48,22 +48,7 @@
     <t xml:space="preserve">Trama_Completa</t>
   </si>
   <si>
-    <t xml:space="preserve">18412345000217701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23138343132333435303030323137373031303330333d00000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">184123450000171300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18412345000017130000000000</t>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
@@ -515,13 +500,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="B1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -591,29 +576,14 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fixed Error in the previous commit
</commit_message>
<xml_diff>
--- a/Ed_FInsOmron/resources/LoggingNormon.xlsx
+++ b/Ed_FInsOmron/resources/LoggingNormon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t xml:space="preserve">DataV10</t>
   </si>
@@ -48,7 +48,73 @@
     <t xml:space="preserve">Trama_Completa</t>
   </si>
   <si>
+    <t xml:space="preserve">18412345000217701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23138343132333435303030323137373031303330333d00000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450000171300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345000017130000000000</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1841234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1841234500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1841234500021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345000217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184123450002177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1841234500021770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18412345000217701030</t>
   </si>
 </sst>
 </file>
@@ -500,13 +566,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="B1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -576,14 +642,32 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>